<commit_message>
added dummy columns for UC effects for all outcomes
MCS, PCS, GHQ36 and GHQ caseness
</commit_message>
<xml_diff>
--- a/input/reg_health_mental.xlsx
+++ b/input/reg_health_mental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF27609-5500-4E8F-A059-053D7C9F8DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC491EDB-607A-4A8A-BFE1-DBE864B901E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="60">
   <si>
     <t>Date modified</t>
   </si>
@@ -202,6 +202,24 @@
   </si>
   <si>
     <t>Dcpst_PreviouslyPartnered_L1</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_ZERO</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_TEN</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_TWENTY</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_THIRTY</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_FORTY</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC</t>
   </si>
 </sst>
 </file>
@@ -3898,16 +3916,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35101A52-F636-4EA1-B514-C92ACE822888}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3944,8 +3964,26 @@
       <c r="L1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3982,8 +4020,26 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4020,8 +4076,26 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4058,8 +4132,26 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4096,8 +4188,26 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -4134,8 +4244,26 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4172,8 +4300,26 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -4210,8 +4356,26 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -4248,80 +4412,470 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B16" s="4">
         <v>0.7547488</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
         <v>2.0778007724100004E-3</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B17" s="4">
         <v>6.9100000000000003E-3</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" s="6">
         <v>2.0550899556099999E-3</v>
       </c>
     </row>
@@ -4333,16 +4887,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83C27E0-FA2B-440E-9BE2-866FFC98D161}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4379,8 +4935,26 @@
       <c r="L1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4417,8 +4991,26 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4455,8 +5047,26 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4493,8 +5103,26 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4531,8 +5159,26 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -4569,8 +5215,26 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4607,8 +5271,26 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -4645,8 +5327,26 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -4683,80 +5383,470 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B16" s="4">
         <v>0.7547488</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
         <v>2.0778007724100004E-3</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B17" s="4">
         <v>6.9100000000000003E-3</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" s="6">
         <v>2.0550899556099999E-3</v>
       </c>
     </row>
@@ -4769,7 +5859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C367505C-FD84-46B3-9749-6444C1C58A26}">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -7637,9 +8727,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90524CD9-FC25-43D3-A993-DE235AB6CC61}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7647,7 +8739,7 @@
     <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -7678,8 +8770,26 @@
       <c r="J1" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -7710,8 +8820,26 @@
       <c r="J2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -7742,8 +8870,26 @@
       <c r="J3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -7774,8 +8920,26 @@
       <c r="J4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -7806,8 +8970,26 @@
       <c r="J5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -7838,8 +9020,26 @@
       <c r="J6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -7870,8 +9070,26 @@
       <c r="J7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>41</v>
       </c>
@@ -7902,8 +9120,26 @@
       <c r="J8" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
@@ -7933,6 +9169,324 @@
       </c>
       <c r="J9" s="8">
         <v>4.7043339317226502E-3</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7943,9 +9497,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC91F47-2228-4CD9-A074-8E6E16867A5F}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7953,7 +9509,7 @@
     <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -7984,8 +9540,26 @@
       <c r="J1" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -8016,8 +9590,26 @@
       <c r="J2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -8048,8 +9640,26 @@
       <c r="J3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -8080,8 +9690,26 @@
       <c r="J4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -8112,8 +9740,26 @@
       <c r="J5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -8144,8 +9790,26 @@
       <c r="J6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -8176,8 +9840,26 @@
       <c r="J7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>41</v>
       </c>
@@ -8208,8 +9890,26 @@
       <c r="J8" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
@@ -8239,6 +9939,324 @@
       </c>
       <c r="J9" s="8">
         <v>4.4853158471408801E-3</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UC flat effects applied
</commit_message>
<xml_diff>
--- a/input/reg_health_mental.xlsx
+++ b/input/reg_health_mental.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC491EDB-607A-4A8A-BFE1-DBE864B901E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46220635-BFE1-4E74-AC54-FCD8B2863DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3919,7 +3919,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="B15" sqref="B15:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4716,7 +4716,7 @@
         <v>59</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.312</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -4758,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>2.3408999999999999E-2</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -4890,7 +4890,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5687,7 +5687,7 @@
         <v>59</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.312</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -5729,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>2.3408999999999999E-2</v>
       </c>
       <c r="Q15">
         <v>0</v>

</xml_diff>